<commit_message>
Adding tasks of week 2
</commit_message>
<xml_diff>
--- a/Planning/CAR_ RACI.xlsx
+++ b/Planning/CAR_ RACI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\SARA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\CarPurchasing\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="53">
   <si>
     <t>CAR_RACI</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Project Manager Name:</t>
   </si>
   <si>
-    <t>Sarah Ibrahim</t>
-  </si>
-  <si>
     <t>Project Description:</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Issue sheet Review</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>SIQ</t>
   </si>
   <si>
@@ -135,14 +129,62 @@
     <t>CM Training</t>
   </si>
   <si>
-    <t>A</t>
+    <t>HLD Review</t>
+  </si>
+  <si>
+    <t>DFD</t>
+  </si>
+  <si>
+    <t>DFD Review</t>
+  </si>
+  <si>
+    <t>UML Class Diagram</t>
+  </si>
+  <si>
+    <t>UML Class Diagram Review</t>
+  </si>
+  <si>
+    <t>UML Use Case</t>
+  </si>
+  <si>
+    <t>UML Use Case Review</t>
+  </si>
+  <si>
+    <t>Design Doc</t>
+  </si>
+  <si>
+    <t>Sara Ibrahim</t>
+  </si>
+  <si>
+    <t>UML Sequence</t>
+  </si>
+  <si>
+    <t>UML Sequence Review</t>
+  </si>
+  <si>
+    <t>Updated Project Plan</t>
+  </si>
+  <si>
+    <t>Updated Project Plan Review</t>
+  </si>
+  <si>
+    <t>Updated SRS</t>
+  </si>
+  <si>
+    <t>Updated SRS Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLD </t>
+  </si>
+  <si>
+    <t>Design Doc Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,11 +203,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
     </font>
@@ -174,19 +211,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
@@ -196,49 +222,57 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -273,70 +307,1664 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="204">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FC5E8"/>
+          <bgColor rgb="FF9FC5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -645,16 +2273,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1004"/>
+  <dimension ref="A1:Y1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -668,13 +2296,13 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -693,119 +2321,119 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="18.75">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="32.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:25" ht="18.75">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
+      <c r="B3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" ht="18.75">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:25" ht="35.25" customHeight="1">
+      <c r="A4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" ht="18.75">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -826,558 +2454,911 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:25" ht="15.75">
+      <c r="A6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="C7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:25" ht="15.75">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="D8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:25" ht="15.75">
+      <c r="A9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="A9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="F9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:25" ht="27.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:25" ht="15.75">
+      <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="C11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.75">
+      <c r="A12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75">
+      <c r="A13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75">
+      <c r="A14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="D14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="16"/>
     </row>
-    <row r="11" spans="1:25">
-      <c r="A11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="12" t="s">
+    <row r="15" spans="1:25" ht="15.75">
+      <c r="A15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:25" ht="15.75">
+      <c r="A16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="G16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75">
+      <c r="A17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="D17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75">
+      <c r="A18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="C18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75">
+      <c r="A19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
+      <c r="H19" s="11"/>
     </row>
-    <row r="12" spans="1:25">
-      <c r="A12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="15" t="s">
+    <row r="20" spans="1:13" ht="15.75">
+      <c r="A20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75">
+      <c r="A21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="G21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75">
+      <c r="A22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="18"/>
+      <c r="H23" s="11"/>
     </row>
-    <row r="13" spans="1:25">
-      <c r="A13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="12" t="s">
+    <row r="24" spans="1:13" ht="15.75">
+      <c r="A24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="A16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="F24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="F25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" s="10" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" s="10" customFormat="1" ht="15.75">
+      <c r="A27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="24"/>
+      <c r="D27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="24"/>
-      <c r="M28" s="25" t="s">
-        <v>16</v>
-      </c>
+      <c r="A28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="11"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="M29" s="25" t="s">
-        <v>38</v>
-      </c>
+      <c r="A29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="24"/>
-      <c r="M30" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="A30" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="24"/>
-      <c r="M31" s="25" t="s">
+      <c r="A31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="C31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="24"/>
+      <c r="A32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="M32" s="8"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A33" s="24"/>
+    <row r="33" spans="1:13" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="11"/>
+      <c r="M33" s="8"/>
     </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A34" s="24"/>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A34" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A35" s="24"/>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A35" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A36" s="24"/>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A36" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A37" s="24"/>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A37" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A38" s="24"/>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A38" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A39" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A40" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A41" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A42" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2332,8 +4313,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E1:I1"/>
@@ -2341,32 +4320,512 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:G40">
+  <conditionalFormatting sqref="B39:D39 F39:G39 E40 B6:G25 B28:G38">
+    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:D39 F39:G39 E40 B6:G25 B28:G38">
+    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:D39 F39:G39 E40 B6:G25 B28:G38">
+    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:D39 F39:G39 E40 B6:G25 B28:G38">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="92" priority="104" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="cellIs" dxfId="87" priority="93" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="83" priority="89" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="82" priority="90" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="81" priority="91" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="80" priority="92" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="79" priority="29" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="78" priority="30" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="77" priority="31" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="76" priority="32" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="75" priority="81" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="71" priority="77" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="70" priority="78" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="69" priority="79" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="68" priority="80" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="67" priority="41" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="65" priority="43" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="64" priority="44" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="cellIs" dxfId="52" priority="64" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="cellIs" dxfId="40" priority="52" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"I"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G40">
+  <conditionalFormatting sqref="B27">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G40">
+  <conditionalFormatting sqref="B27">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G40">
+  <conditionalFormatting sqref="B27">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B6:G46">
-      <formula1>$M$28:$M$31</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="B6:G25 B27:G44">
+      <formula1>$M$29:$M$32</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>